<commit_message>
Legs and Rooms Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 2/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 2/automatic calibration calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub\New 2\Sesi 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub2\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +797,7 @@
         <v>1500</v>
       </c>
       <c r="D8" s="1">
-        <v>1280</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="1">
         <v>1900</v>
@@ -810,7 +810,7 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
DNM Fixing Legs Sesi 1,2 and 3!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 2/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 2/automatic calibration calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAB57F4-BB50-48AC-B885-175EC96BACC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105AECF1-313F-4C1F-8188-3E461718F91E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
         <v>1400</v>
       </c>
       <c r="C6" s="1">
-        <v>1280</v>
+        <v>1180</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
@@ -716,18 +716,18 @@
         <v>850</v>
       </c>
       <c r="F6" s="1">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="G6" s="1">
-        <v>2180</v>
+        <v>2150</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2680</v>
+        <v>2620</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1280</v>
+        <v>1180</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,7 +735,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>-470</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>

</xml_diff>